<commit_message>
New diagrams fixs, Relatorio updates
</commit_message>
<xml_diff>
--- a/docs/Requisitos.xlsx
+++ b/docs/Requisitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WallQ-\Documents\GitHub\Basicamente\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C747D2E-E0AF-4BB7-B9DD-BF0A337903F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185C8C69-18F7-4EA9-BAE5-0CC5C36B9995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{38A5A072-F1EA-442E-B2D3-7554C672FC8C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t>Descrição</t>
   </si>
@@ -60,9 +60,6 @@
   <si>
     <t>Urgente - SIM
 Importante -SIM</t>
-  </si>
-  <si>
-    <t>Qualquer utilizador</t>
   </si>
   <si>
     <t>N/A</t>
@@ -138,15 +135,9 @@
     <t>RNF-004: Desempenho</t>
   </si>
   <si>
-    <t>Devem ser tidos em conta formas de melhorar de a performance da aplicação, sejá através do uso de imagens com formato .webp e loading do tipo lazy, a bundles de .css, .js, purgados e minificados de forma a reduzir o payload de cada request, etc…</t>
-  </si>
-  <si>
     <t>RI-001: Tipografia</t>
   </si>
   <si>
-    <t>O tamanho da fonte não deve ser menor que 0.875rem/14px.</t>
-  </si>
-  <si>
     <t>RI-002:  Acessibilidade</t>
   </si>
   <si>
@@ -163,6 +154,56 @@
   </si>
   <si>
     <t>RF-002: Contactar</t>
+  </si>
+  <si>
+    <t>O tipo de letra deve ser Poppins e o tamanho da fonte não deve ser menor que 0.875rem/14px.</t>
+  </si>
+  <si>
+    <t>RNF-005: Compatibilidade</t>
+  </si>
+  <si>
+    <t>A aplicação deve ser completamente funcional sem muita discrepância de web browser para web browser.</t>
+  </si>
+  <si>
+    <t>Devem ser tidos em conta formas de melhorar de a performance da aplicação e o SEO, sejá através do uso de imagens com formato .webp e loading do tipo lazy, a bundles de .css, .js, purgados e minificados de forma a reduzir o payload de cada request, etc…</t>
+  </si>
+  <si>
+    <t>RF-003: Mudar linguagem</t>
+  </si>
+  <si>
+    <t>Esta funcionalidade permite ao utilizador alterar entre português e inglês o conteúdo apresentado.</t>
+  </si>
+  <si>
+    <t>Urgente - NÃO
+Importante -SIM</t>
+  </si>
+  <si>
+    <t>Esta funcionalidade permite ao utilizador através de um botão voltar para o topo da página.</t>
+  </si>
+  <si>
+    <t>Urgente - NÃO
+Importante -NÃO</t>
+  </si>
+  <si>
+    <t>Apenas deverá ficar visível apos serem movidos no eixo Y 300 pixeis.</t>
+  </si>
+  <si>
+    <t>Utilizador anónimo</t>
+  </si>
+  <si>
+    <t>RF-004: Voltar para o topo</t>
+  </si>
+  <si>
+    <t>RI-004:  Cor</t>
+  </si>
+  <si>
+    <t>O formato das imagens deve ser do tipo webp.</t>
+  </si>
+  <si>
+    <t>As cores devem estar em conformidade da basicamente, ou seja, branco(#ffffff) e azul(#0c5eac).</t>
+  </si>
+  <si>
+    <t>RI-005:  Formato de imagens</t>
   </si>
 </sst>
 </file>
@@ -357,46 +398,46 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -713,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E098CD-7BC0-45E9-82D0-8965FB48D57B}">
-  <dimension ref="B1:Y26"/>
+  <dimension ref="B1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,28 +786,28 @@
       <c r="Y1" s="8"/>
     </row>
     <row r="2" spans="2:25" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-      <c r="H2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="H2" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
       <c r="M2" s="7"/>
-      <c r="N2" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
+      <c r="N2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="8"/>
@@ -779,31 +820,31 @@
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
       <c r="H3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="I3" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
       <c r="M3" s="7"/>
       <c r="N3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
+      <c r="O3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="8"/>
@@ -816,17 +857,17 @@
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
       <c r="M4" s="7"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -845,27 +886,27 @@
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-      <c r="H5" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
+      <c r="C5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
+      <c r="H5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
       <c r="M5" s="7"/>
-      <c r="N5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
+      <c r="N5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
       <c r="U5" s="8"/>
@@ -878,31 +919,31 @@
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
+      <c r="C6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
       <c r="H6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="I6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
       <c r="M6" s="7"/>
       <c r="N6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="O6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
+      <c r="O6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
       <c r="U6" s="8"/>
@@ -915,17 +956,17 @@
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
+      <c r="C7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
       <c r="M7" s="7"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
@@ -941,21 +982,21 @@
       <c r="Y7" s="8"/>
     </row>
     <row r="8" spans="2:25" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H8" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
+      <c r="H8" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="N8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
       <c r="U8" s="8"/>
@@ -965,32 +1006,32 @@
       <c r="Y8" s="8"/>
     </row>
     <row r="9" spans="2:25" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
+      <c r="B9" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
       <c r="H9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
+      <c r="I9" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
       <c r="M9" s="7"/>
       <c r="N9" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="O9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
+      <c r="O9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
       <c r="U9" s="8"/>
@@ -1003,12 +1044,12 @@
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
+      <c r="C10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -1032,25 +1073,27 @@
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
-      <c r="H11" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="H11" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
+      <c r="N11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="8"/>
@@ -1063,27 +1106,31 @@
       <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
+      <c r="C12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
       <c r="H12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="I12" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
+      <c r="N12" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="8"/>
@@ -1096,12 +1143,12 @@
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="24"/>
+      <c r="C13" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
@@ -1125,23 +1172,27 @@
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="C14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="H14" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
       <c r="M14" s="7"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
+      <c r="N14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
       <c r="U14" s="8"/>
@@ -1150,23 +1201,31 @@
       <c r="X14" s="8"/>
       <c r="Y14" s="8"/>
     </row>
-    <row r="15" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
+      <c r="H15" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
       <c r="M15" s="7"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
+      <c r="N15" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
       <c r="U15" s="8"/>
@@ -1175,12 +1234,14 @@
       <c r="X15" s="8"/>
       <c r="Y15" s="8"/>
     </row>
-    <row r="16" spans="2:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+    <row r="16" spans="2:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -1200,23 +1261,22 @@
       <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
     </row>
-    <row r="17" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+    <row r="17" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="U17" s="8"/>
@@ -1225,23 +1285,22 @@
       <c r="X17" s="8"/>
       <c r="Y17" s="8"/>
     </row>
-    <row r="18" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+    <row r="18" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
       <c r="U18" s="8"/>
@@ -1250,12 +1309,16 @@
       <c r="X18" s="8"/>
       <c r="Y18" s="8"/>
     </row>
-    <row r="19" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+    <row r="19" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -1275,12 +1338,16 @@
       <c r="X19" s="8"/>
       <c r="Y19" s="8"/>
     </row>
-    <row r="20" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+    <row r="20" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -1300,12 +1367,16 @@
       <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
     </row>
-    <row r="21" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+    <row r="21" spans="2:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -1325,7 +1396,7 @@
       <c r="X21" s="8"/>
       <c r="Y21" s="8"/>
     </row>
-    <row r="22" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -1345,7 +1416,14 @@
       <c r="X22" s="8"/>
       <c r="Y22" s="8"/>
     </row>
-    <row r="23" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="18"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -1365,7 +1443,16 @@
       <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
     </row>
-    <row r="24" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -1385,7 +1472,16 @@
       <c r="X24" s="8"/>
       <c r="Y24" s="8"/>
     </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
@@ -1400,7 +1496,16 @@
       <c r="X25" s="8"/>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
       <c r="U26" s="8"/>
@@ -1409,36 +1514,76 @@
       <c r="X26" s="8"/>
       <c r="Y26" s="8"/>
     </row>
+    <row r="27" spans="2:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="21"/>
+    </row>
+    <row r="28" spans="2:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
+  <mergeCells count="46">
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="O9:R9"/>
     <mergeCell ref="I12:L12"/>
-    <mergeCell ref="H11:L11"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="I6:L6"/>
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="H5:L5"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="N8:R8"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="O12:R12"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="H11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>